<commit_message>
excel parser bug fixed
</commit_message>
<xml_diff>
--- a/config/excel/att.xlsx
+++ b/config/excel/att.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>待定</t>
   </si>
@@ -54,18 +54,9 @@
     <t>蓝量</t>
   </si>
   <si>
-    <t>物理攻击力</t>
-  </si>
-  <si>
     <t>物理防御力</t>
   </si>
   <si>
-    <t>魔法攻击力</t>
-  </si>
-  <si>
-    <t>魔法防御力</t>
-  </si>
-  <si>
     <t>暴击率</t>
   </si>
   <si>
@@ -111,16 +102,7 @@
     <t>MaxMP</t>
   </si>
   <si>
-    <t>Atn</t>
-  </si>
-  <si>
     <t>Def</t>
-  </si>
-  <si>
-    <t>Ats</t>
-  </si>
-  <si>
-    <t>Adf</t>
   </si>
   <si>
     <t>CriProb</t>
@@ -221,6 +203,14 @@
   </si>
   <si>
     <t>0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Atk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击力</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1609,10 +1599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V17"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1624,19 +1614,19 @@
     <col min="5" max="8" width="7.25" style="1" customWidth="1"/>
     <col min="9" max="9" width="7.875" style="1" customWidth="1"/>
     <col min="10" max="11" width="7.25" style="1" customWidth="1"/>
-    <col min="12" max="15" width="8.375" style="1" customWidth="1"/>
+    <col min="12" max="13" width="8.375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.375" style="1" customWidth="1"/>
     <col min="16" max="16" width="11.875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="8.375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="9.625" style="1" customWidth="1"/>
-    <col min="20" max="22" width="11.875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="9" style="1"/>
+    <col min="17" max="17" width="9.625" style="1" customWidth="1"/>
+    <col min="18" max="20" width="11.875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="9" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1650,7 +1640,9 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="N1" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="O1" s="3"/>
       <c r="P1" s="2" t="s">
         <v>0</v>
@@ -1659,18 +1651,14 @@
       <c r="R1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="3"/>
+      <c r="S1" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="T1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="2" spans="1:22" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
@@ -1686,7 +1674,9 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="N2" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="O2" s="4"/>
       <c r="P2" s="5" t="s">
         <v>2</v>
@@ -1695,86 +1685,76 @@
       <c r="R2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="4"/>
+      <c r="S2" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="T2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="U2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="3" spans="1:22" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="L3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="Q3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="R3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="T3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="V3" s="8" t="s">
-        <v>40</v>
-      </c>
     </row>
-    <row r="4" spans="1:22" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>3</v>
@@ -1801,175 +1781,157 @@
         <v>10</v>
       </c>
       <c r="L4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="P4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="Q4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="R4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="S4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="T4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="T4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="V4" s="8" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="5" spans="1:22" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="T5" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="V5" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="M6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="O6" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="T6" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="V6" s="8" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:20" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="10">
         <v>1</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E7" s="12">
         <v>100</v>
@@ -1999,41 +1961,35 @@
         <v>100</v>
       </c>
       <c r="N7" s="12">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="O7" s="12">
-        <v>20</v>
+        <v>1200</v>
       </c>
       <c r="P7" s="12">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="Q7" s="12">
+        <v>0</v>
+      </c>
+      <c r="R7" s="12">
         <v>1200</v>
       </c>
-      <c r="R7" s="12">
+      <c r="S7" s="12">
         <v>10000</v>
       </c>
-      <c r="S7" s="12">
+      <c r="T7" s="12">
         <v>0</v>
       </c>
-      <c r="T7" s="12">
-        <v>1200</v>
-      </c>
-      <c r="U7" s="12">
-        <v>10000</v>
-      </c>
-      <c r="V7" s="12">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:20" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="13">
         <v>2</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E8" s="15">
         <v>12</v>
@@ -2063,41 +2019,35 @@
         <v>60</v>
       </c>
       <c r="N8" s="15">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="O8" s="15">
-        <v>100</v>
+        <v>1300</v>
       </c>
       <c r="P8" s="15">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="Q8" s="15">
+        <v>0</v>
+      </c>
+      <c r="R8" s="15">
         <v>1300</v>
       </c>
-      <c r="R8" s="15">
+      <c r="S8" s="15">
         <v>10000</v>
       </c>
-      <c r="S8" s="15">
+      <c r="T8" s="15">
         <v>0</v>
       </c>
-      <c r="T8" s="15">
-        <v>1300</v>
-      </c>
-      <c r="U8" s="15">
-        <v>10000</v>
-      </c>
-      <c r="V8" s="15">
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:20" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="13">
         <v>3</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E9" s="15">
         <v>11</v>
@@ -2130,38 +2080,32 @@
         <v>100</v>
       </c>
       <c r="O9" s="15">
-        <v>120</v>
+        <v>1400</v>
       </c>
       <c r="P9" s="15">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="Q9" s="15">
+        <v>0</v>
+      </c>
+      <c r="R9" s="15">
         <v>1400</v>
       </c>
-      <c r="R9" s="15">
+      <c r="S9" s="15">
         <v>10000</v>
       </c>
-      <c r="S9" s="15">
+      <c r="T9" s="15">
         <v>0</v>
       </c>
-      <c r="T9" s="15">
-        <v>1400</v>
-      </c>
-      <c r="U9" s="15">
-        <v>10000</v>
-      </c>
-      <c r="V9" s="15">
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:20" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="13">
         <v>4</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E10" s="15">
         <v>100</v>
@@ -2191,41 +2135,35 @@
         <v>100</v>
       </c>
       <c r="N10" s="15">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="O10" s="15">
-        <v>20</v>
+        <v>1500</v>
       </c>
       <c r="P10" s="15">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="Q10" s="15">
+        <v>1000</v>
+      </c>
+      <c r="R10" s="15">
         <v>1500</v>
       </c>
-      <c r="R10" s="15">
+      <c r="S10" s="15">
         <v>5000</v>
       </c>
-      <c r="S10" s="15">
+      <c r="T10" s="15">
         <v>1000</v>
       </c>
-      <c r="T10" s="15">
-        <v>1500</v>
-      </c>
-      <c r="U10" s="15">
-        <v>5000</v>
-      </c>
-      <c r="V10" s="15">
-        <v>1000</v>
-      </c>
     </row>
-    <row r="11" spans="1:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:20" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="13">
         <v>5</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E11" s="15">
         <v>189</v>
@@ -2255,41 +2193,35 @@
         <v>140</v>
       </c>
       <c r="N11" s="15">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="O11" s="15">
-        <v>20</v>
+        <v>1600</v>
       </c>
       <c r="P11" s="15">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="Q11" s="15">
+        <v>0</v>
+      </c>
+      <c r="R11" s="15">
         <v>1600</v>
       </c>
-      <c r="R11" s="15">
+      <c r="S11" s="15">
         <v>10000</v>
       </c>
-      <c r="S11" s="15">
+      <c r="T11" s="15">
         <v>0</v>
       </c>
-      <c r="T11" s="15">
-        <v>1600</v>
-      </c>
-      <c r="U11" s="15">
-        <v>10000</v>
-      </c>
-      <c r="V11" s="15">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:20" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="13">
         <v>6</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E12" s="15">
         <v>278</v>
@@ -2319,41 +2251,35 @@
         <v>180</v>
       </c>
       <c r="N12" s="15">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="O12" s="15">
-        <v>100</v>
+        <v>1700</v>
       </c>
       <c r="P12" s="15">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="Q12" s="15">
+        <v>0</v>
+      </c>
+      <c r="R12" s="15">
         <v>1700</v>
       </c>
-      <c r="R12" s="15">
+      <c r="S12" s="15">
         <v>10000</v>
       </c>
-      <c r="S12" s="15">
+      <c r="T12" s="15">
         <v>0</v>
       </c>
-      <c r="T12" s="15">
-        <v>1700</v>
-      </c>
-      <c r="U12" s="15">
-        <v>10000</v>
-      </c>
-      <c r="V12" s="15">
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:20" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="13">
         <v>7</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E13" s="15">
         <v>367</v>
@@ -2386,38 +2312,32 @@
         <v>100</v>
       </c>
       <c r="O13" s="15">
-        <v>120</v>
+        <v>1800</v>
       </c>
       <c r="P13" s="15">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="Q13" s="15">
+        <v>0</v>
+      </c>
+      <c r="R13" s="15">
         <v>1800</v>
       </c>
-      <c r="R13" s="15">
+      <c r="S13" s="15">
         <v>10000</v>
       </c>
-      <c r="S13" s="15">
+      <c r="T13" s="15">
         <v>0</v>
       </c>
-      <c r="T13" s="15">
-        <v>1800</v>
-      </c>
-      <c r="U13" s="15">
-        <v>10000</v>
-      </c>
-      <c r="V13" s="15">
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:20" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="13">
         <v>8</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E14" s="15">
         <v>456</v>
@@ -2447,41 +2367,35 @@
         <v>260</v>
       </c>
       <c r="N14" s="15">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="O14" s="15">
-        <v>20</v>
+        <v>1900</v>
       </c>
       <c r="P14" s="15">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="Q14" s="15">
+        <v>1000</v>
+      </c>
+      <c r="R14" s="15">
         <v>1900</v>
       </c>
-      <c r="R14" s="15">
+      <c r="S14" s="15">
         <v>5000</v>
       </c>
-      <c r="S14" s="15">
+      <c r="T14" s="15">
         <v>1000</v>
       </c>
-      <c r="T14" s="15">
-        <v>1900</v>
-      </c>
-      <c r="U14" s="15">
-        <v>5000</v>
-      </c>
-      <c r="V14" s="15">
-        <v>1000</v>
-      </c>
     </row>
-    <row r="15" spans="1:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:20" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="13">
         <v>9</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E15" s="15">
         <v>545</v>
@@ -2511,41 +2425,35 @@
         <v>300</v>
       </c>
       <c r="N15" s="15">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="O15" s="15">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="P15" s="15">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="Q15" s="15">
+        <v>0</v>
+      </c>
+      <c r="R15" s="15">
         <v>2000</v>
       </c>
-      <c r="R15" s="15">
+      <c r="S15" s="15">
         <v>10000</v>
       </c>
-      <c r="S15" s="15">
+      <c r="T15" s="15">
         <v>0</v>
       </c>
-      <c r="T15" s="15">
-        <v>2000</v>
-      </c>
-      <c r="U15" s="15">
-        <v>10000</v>
-      </c>
-      <c r="V15" s="15">
-        <v>0</v>
-      </c>
     </row>
-    <row r="16" spans="1:22" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:20" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="13">
         <v>10</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E16" s="15">
         <v>634</v>
@@ -2575,34 +2483,28 @@
         <v>340</v>
       </c>
       <c r="N16" s="15">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="O16" s="15">
-        <v>100</v>
+        <v>2100</v>
       </c>
       <c r="P16" s="15">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="Q16" s="15">
+        <v>0</v>
+      </c>
+      <c r="R16" s="15">
         <v>2100</v>
       </c>
-      <c r="R16" s="15">
+      <c r="S16" s="15">
         <v>10000</v>
       </c>
-      <c r="S16" s="15">
+      <c r="T16" s="15">
         <v>0</v>
       </c>
-      <c r="T16" s="15">
-        <v>2100</v>
-      </c>
-      <c r="U16" s="15">
-        <v>10000</v>
-      </c>
-      <c r="V16" s="15">
-        <v>0</v>
-      </c>
     </row>
-    <row r="17" spans="1:22" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="6"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -2619,12 +2521,10 @@
       <c r="N17" s="16"/>
       <c r="O17" s="16"/>
       <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
       <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>